<commit_message>
Ajuste de criterio entre vueltas
</commit_message>
<xml_diff>
--- a/Simulador/res_sim.xlsx
+++ b/Simulador/res_sim.xlsx
@@ -435,16 +435,16 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>210.7721984154128</v>
+        <v>217.3237578947572</v>
       </c>
       <c r="D2">
-        <v>26.7703685760498</v>
+        <v>27.18445777893066</v>
       </c>
       <c r="E2">
         <v>344.0415503671599</v>
       </c>
       <c r="F2">
-        <v>46.26569366455078</v>
+        <v>45.56094360351562</v>
       </c>
       <c r="G2">
         <v>1.596116034322399</v>
@@ -453,7 +453,7 @@
         <v>3.492272793926644</v>
       </c>
       <c r="I2">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -464,16 +464,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>198.5145536995319</v>
+        <v>195.8442626255413</v>
       </c>
       <c r="D3">
-        <v>34.89839172363281</v>
+        <v>34.72961807250977</v>
       </c>
       <c r="E3">
         <v>13.56729663011254</v>
       </c>
       <c r="F3">
-        <v>1.399556398391724</v>
+        <v>1.406357765197754</v>
       </c>
       <c r="G3">
         <v>-0.2188322408916709</v>
@@ -482,7 +482,7 @@
         <v>1.57454844203958</v>
       </c>
       <c r="I3">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -493,16 +493,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>207.6413092108305</v>
+        <v>204.7596666005107</v>
       </c>
       <c r="D4">
-        <v>32.52976226806641</v>
+        <v>32.34762954711914</v>
       </c>
       <c r="E4">
         <v>168.9935131340457</v>
       </c>
       <c r="F4">
-        <v>18.7021541595459</v>
+        <v>18.80745697021484</v>
       </c>
       <c r="G4">
         <v>0.3711593507547151</v>
@@ -511,7 +511,7 @@
         <v>1.731397461341183</v>
       </c>
       <c r="I4">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -522,16 +522,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>199.9137848257901</v>
+        <v>201.2765503290809</v>
       </c>
       <c r="D5">
-        <v>34.22743606567383</v>
+        <v>34.31356811523438</v>
       </c>
       <c r="E5">
         <v>17.33180625774378</v>
       </c>
       <c r="F5">
-        <v>1.822938084602356</v>
+        <v>1.818362474441528</v>
       </c>
       <c r="G5">
         <v>-0.0675955599860016</v>
@@ -540,7 +540,7 @@
         <v>1.57520843538257</v>
       </c>
       <c r="I5">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -551,16 +551,16 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>201.0569887680481</v>
+        <v>198.2803155278839</v>
       </c>
       <c r="D6">
-        <v>33.7899284362793</v>
+        <v>33.61442947387695</v>
       </c>
       <c r="E6">
         <v>48.49833201473393</v>
       </c>
       <c r="F6">
-        <v>5.16704273223877</v>
+        <v>5.194019317626953</v>
       </c>
       <c r="G6">
         <v>0.07414374889212304</v>
@@ -569,7 +569,7 @@
         <v>3.40763809526817</v>
       </c>
       <c r="I6">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -580,16 +580,16 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>200.8256496118935</v>
+        <v>202.1976258705994</v>
       </c>
       <c r="D7">
-        <v>34.16865158081055</v>
+        <v>34.2553596496582</v>
       </c>
       <c r="E7">
         <v>15.03489657772798</v>
       </c>
       <c r="F7">
-        <v>1.584072709083557</v>
+        <v>1.580062985420227</v>
       </c>
       <c r="G7">
         <v>-0.01674270518462065</v>
@@ -598,7 +598,7 @@
         <v>2.835582102804634</v>
       </c>
       <c r="I7">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -609,16 +609,16 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>179.9555048422345</v>
+        <v>194.1475424770782</v>
       </c>
       <c r="D8">
-        <v>31.73354911804199</v>
+        <v>32.63055419921875</v>
       </c>
       <c r="E8">
         <v>55.21180257348544</v>
       </c>
       <c r="F8">
-        <v>6.263481616973877</v>
+        <v>6.091300010681152</v>
       </c>
       <c r="G8">
         <v>0.2477469273428186</v>
@@ -627,7 +627,7 @@
         <v>4.760357197651417</v>
       </c>
       <c r="I8">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -638,16 +638,16 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>158.2229001722121</v>
+        <v>149.9973501570169</v>
       </c>
       <c r="D9">
-        <v>42.94607925415039</v>
+        <v>42.5806770324707</v>
       </c>
       <c r="E9">
         <v>560.0692098765884</v>
       </c>
       <c r="F9">
-        <v>46.94838333129883</v>
+        <v>47.35127258300781</v>
       </c>
       <c r="G9">
         <v>-2.435372970096637</v>
@@ -656,7 +656,7 @@
         <v>3.98256430003651</v>
       </c>
       <c r="I9">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -667,16 +667,16 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>242.6350322185753</v>
+        <v>249.5719941049813</v>
       </c>
       <c r="D10">
-        <v>24.42939376831055</v>
+        <v>24.86376190185547</v>
       </c>
       <c r="E10">
         <v>1382.447533600548</v>
       </c>
       <c r="F10">
-        <v>203.7222442626953</v>
+        <v>200.1632385253906</v>
       </c>
       <c r="G10">
         <v>2.353631628237696</v>
@@ -685,7 +685,7 @@
         <v>-3.902847856084686</v>
       </c>
       <c r="I10">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -696,16 +696,16 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>212.9316376167789</v>
+        <v>210.2419714782921</v>
       </c>
       <c r="D11">
-        <v>34.99647521972656</v>
+        <v>34.82646942138672</v>
       </c>
       <c r="E11">
         <v>199.1265320145867</v>
       </c>
       <c r="F11">
-        <v>20.4836483001709</v>
+        <v>20.58363914489746</v>
       </c>
       <c r="G11">
         <v>-0.1659918344285073</v>
@@ -714,7 +714,7 @@
         <v>-3.39453113286161</v>
       </c>
       <c r="I11">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -725,16 +725,16 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>215.4457893494151</v>
+        <v>214.0264894498923</v>
       </c>
       <c r="D12">
-        <v>33.14532852172852</v>
+        <v>33.05561828613281</v>
       </c>
       <c r="E12">
         <v>91.86067101041317</v>
       </c>
       <c r="F12">
-        <v>9.977225303649902</v>
+        <v>10.00430297851562</v>
       </c>
       <c r="G12">
         <v>0.2482922711943954</v>
@@ -743,7 +743,7 @@
         <v>-2.756201684925812</v>
       </c>
       <c r="I12">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -772,7 +772,7 @@
         <v>-0.6139341684454964</v>
       </c>
       <c r="I13">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -783,16 +783,16 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>253.9365500055254</v>
+        <v>248.3795926524217</v>
       </c>
       <c r="D14">
-        <v>20.95455741882324</v>
+        <v>20.65255737304688</v>
       </c>
       <c r="E14">
         <v>1755.103346009126</v>
       </c>
       <c r="F14">
-        <v>301.52734375</v>
+        <v>305.9365539550781</v>
       </c>
       <c r="G14">
         <v>3.32023723483058</v>
@@ -801,7 +801,7 @@
         <v>-2.486692203613646</v>
       </c>
       <c r="I14">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -830,7 +830,7 @@
         <v>-4.904003908876237</v>
       </c>
       <c r="I15">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -859,7 +859,7 @@
         <v>-5.685938728369462</v>
       </c>
       <c r="I16">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -870,16 +870,16 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>166.423424158676</v>
+        <v>164.5624438988838</v>
       </c>
       <c r="D17">
-        <v>41.27479934692383</v>
+        <v>41.17624664306641</v>
       </c>
       <c r="E17">
         <v>778.6626264767738</v>
       </c>
       <c r="F17">
-        <v>67.91517639160156</v>
+        <v>68.07772827148438</v>
       </c>
       <c r="G17">
         <v>-2.347143802750921</v>
@@ -888,7 +888,7 @@
         <v>-5.184267536920604</v>
       </c>
       <c r="I17">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -917,7 +917,7 @@
         <v>-1.272944327177375</v>
       </c>
       <c r="I18">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -928,16 +928,16 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>177.9457954990679</v>
+        <v>177.0045805365757</v>
       </c>
       <c r="D19">
-        <v>41.70973968505859</v>
+        <v>41.65996932983398</v>
       </c>
       <c r="E19">
         <v>2858.371279980439</v>
       </c>
       <c r="F19">
-        <v>246.7082366943359</v>
+        <v>247.0029754638672</v>
       </c>
       <c r="G19">
         <v>-2.290160995983005</v>
@@ -946,7 +946,7 @@
         <v>-4.949172023586057</v>
       </c>
       <c r="I19">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -975,7 +975,7 @@
         <v>-9.70486363213517</v>
       </c>
       <c r="I20">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1004,7 +1004,7 @@
         <v>-9.861219867994032</v>
       </c>
       <c r="I21">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1033,7 +1033,7 @@
         <v>-9.279345091961993</v>
       </c>
       <c r="I22">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1062,7 +1062,7 @@
         <v>-9.238281327998019</v>
       </c>
       <c r="I23">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1091,7 +1091,7 @@
         <v>-9.954147471937697</v>
       </c>
       <c r="I24">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1102,16 +1102,16 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>217.6438962575264</v>
+        <v>191.1916136342531</v>
       </c>
       <c r="D25">
-        <v>34.1511116027832</v>
+        <v>32.48984909057617</v>
       </c>
       <c r="E25">
         <v>229.7816471182123</v>
       </c>
       <c r="F25">
-        <v>24.22216796875</v>
+        <v>25.4606876373291</v>
       </c>
       <c r="G25">
         <v>-0.2558670563346051</v>
@@ -1120,7 +1120,7 @@
         <v>-9.022411740833657</v>
       </c>
       <c r="I25">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1149,7 +1149,7 @@
         <v>-8.465904839481219</v>
       </c>
       <c r="I26">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1178,7 +1178,7 @@
         <v>-9.450384387180872</v>
       </c>
       <c r="I27">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1207,7 +1207,7 @@
         <v>-9.945059851748946</v>
       </c>
       <c r="I28">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1236,7 +1236,7 @@
         <v>-9.385389381431935</v>
       </c>
       <c r="I29">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1247,16 +1247,16 @@
         <v>28</v>
       </c>
       <c r="C30">
-        <v>219.0399198804652</v>
+        <v>223.2098610730541</v>
       </c>
       <c r="D30">
-        <v>33.14225387573242</v>
+        <v>33.40224075317383</v>
       </c>
       <c r="E30">
         <v>40.33251286838276</v>
       </c>
       <c r="F30">
-        <v>4.381024837493896</v>
+        <v>4.346925258636475</v>
       </c>
       <c r="G30">
         <v>0.141437395741504</v>
@@ -1265,7 +1265,7 @@
         <v>-6.42479720367449</v>
       </c>
       <c r="I30">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1276,16 +1276,16 @@
         <v>29</v>
       </c>
       <c r="C31">
-        <v>141.220620039239</v>
+        <v>139.6808095333958</v>
       </c>
       <c r="D31">
-        <v>45.37101745605469</v>
+        <v>45.4494743347168</v>
       </c>
       <c r="E31">
         <v>561.0455563968753</v>
       </c>
       <c r="F31">
-        <v>44.51660919189453</v>
+        <v>44.43976211547852</v>
       </c>
       <c r="G31">
         <v>-3.228726121143762</v>
@@ -1294,7 +1294,7 @@
         <v>4.029840037148754</v>
       </c>
       <c r="I31">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1305,16 +1305,16 @@
         <v>30</v>
       </c>
       <c r="C32">
-        <v>178.8324503300365</v>
+        <v>179.9038145684369</v>
       </c>
       <c r="D32">
-        <v>30.38631439208984</v>
+        <v>30.45403099060059</v>
       </c>
       <c r="E32">
         <v>104.9411033259221</v>
       </c>
       <c r="F32">
-        <v>12.43283176422119</v>
+        <v>12.40518665313721</v>
       </c>
       <c r="G32">
         <v>0.5587509355297379</v>
@@ -1323,7 +1323,7 @@
         <v>7.35038777279619</v>
       </c>
       <c r="I32">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1334,16 +1334,16 @@
         <v>31</v>
       </c>
       <c r="C33">
-        <v>162.3629447299337</v>
+        <v>157.68203392561</v>
       </c>
       <c r="D33">
-        <v>41.41934585571289</v>
+        <v>41.19766235351562</v>
       </c>
       <c r="E33">
         <v>442.239946164329</v>
       </c>
       <c r="F33">
-        <v>38.43768692016602</v>
+        <v>38.6445198059082</v>
       </c>
       <c r="G33">
         <v>-2.31687999893804</v>
@@ -1352,7 +1352,7 @@
         <v>-2.995590014584259</v>
       </c>
       <c r="I33">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1381,7 +1381,7 @@
         <v>1.64528195886503</v>
       </c>
       <c r="I34">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1410,7 +1410,7 @@
         <v>0.03624061437360713</v>
       </c>
       <c r="I35">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1421,16 +1421,16 @@
         <v>34</v>
       </c>
       <c r="C36">
-        <v>256.991843523155</v>
+        <v>255.1095705474378</v>
       </c>
       <c r="D36">
-        <v>19.85684394836426</v>
+        <v>19.75454711914062</v>
       </c>
       <c r="E36">
         <v>1544.238605138566</v>
       </c>
       <c r="F36">
-        <v>279.9669189453125</v>
+        <v>281.4166870117188</v>
       </c>
       <c r="G36">
         <v>3.623477518515383</v>
@@ -1439,7 +1439,7 @@
         <v>-1.280216372607037</v>
       </c>
       <c r="I36">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1468,7 +1468,7 @@
         <v>1.418178375911533</v>
       </c>
       <c r="I37">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1479,16 +1479,16 @@
         <v>36</v>
       </c>
       <c r="C38">
-        <v>206.11444124225</v>
+        <v>221.9048797289773</v>
       </c>
       <c r="D38">
-        <v>32.75628662109375</v>
+        <v>33.74606323242188</v>
       </c>
       <c r="E38">
         <v>30.13365751333913</v>
       </c>
       <c r="F38">
-        <v>3.311766386032104</v>
+        <v>3.2146315574646</v>
       </c>
       <c r="G38">
         <v>0.04705830724490476</v>
@@ -1497,7 +1497,7 @@
         <v>-6.504653418974739</v>
       </c>
       <c r="I38">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1508,16 +1508,16 @@
         <v>37</v>
       </c>
       <c r="C39">
-        <v>206.8557862588803</v>
+        <v>197.9099258641761</v>
       </c>
       <c r="D39">
-        <v>36.10295486450195</v>
+        <v>35.60295104980469</v>
       </c>
       <c r="E39">
         <v>46.67657954138122</v>
       </c>
       <c r="F39">
-        <v>4.654346942901611</v>
+        <v>4.719712257385254</v>
       </c>
       <c r="G39">
         <v>-0.5267327097768739</v>
@@ -1526,7 +1526,7 @@
         <v>-4.414407877173214</v>
       </c>
       <c r="I39">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1555,7 +1555,7 @@
         <v>3.558546856154219</v>
       </c>
       <c r="I40">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1566,16 +1566,16 @@
         <v>39</v>
       </c>
       <c r="C41">
-        <v>194.073620314031</v>
+        <v>195.3906980723375</v>
       </c>
       <c r="D41">
-        <v>35.06266403198242</v>
+        <v>35.14591217041016</v>
       </c>
       <c r="E41">
         <v>340.4292798588431</v>
       </c>
       <c r="F41">
-        <v>34.9530029296875</v>
+        <v>34.87021255493164</v>
       </c>
       <c r="G41">
         <v>-0.3168343342728075</v>
@@ -1584,7 +1584,7 @@
         <v>1.146574443400988</v>
       </c>
       <c r="I41">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1595,16 +1595,16 @@
         <v>40</v>
       </c>
       <c r="C42">
-        <v>194.1939979598018</v>
+        <v>179.9968553268565</v>
       </c>
       <c r="D42">
-        <v>33.25690460205078</v>
+        <v>32.33523559570312</v>
       </c>
       <c r="E42">
         <v>17.42441686837992</v>
       </c>
       <c r="F42">
-        <v>1.886161684989929</v>
+        <v>1.939924120903015</v>
       </c>
       <c r="G42">
         <v>0.2506431481089307</v>
@@ -1613,7 +1613,7 @@
         <v>9.997376345115907</v>
       </c>
       <c r="I42">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1624,16 +1624,16 @@
         <v>41</v>
       </c>
       <c r="C43">
-        <v>170.1119185630267</v>
+        <v>177.9025666447569</v>
       </c>
       <c r="D43">
-        <v>33.19799423217773</v>
+        <v>33.73945236206055</v>
       </c>
       <c r="E43">
         <v>17.19116230919826</v>
       </c>
       <c r="F43">
-        <v>1.864214420318604</v>
+        <v>1.834297180175781</v>
       </c>
       <c r="G43">
         <v>-0.08132546284821182</v>
@@ -1642,7 +1642,7 @@
         <v>9.135520449007458</v>
       </c>
       <c r="I43">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1653,16 +1653,16 @@
         <v>42</v>
       </c>
       <c r="C44">
-        <v>243.8185284348215</v>
+        <v>249.3489983864139</v>
       </c>
       <c r="D44">
-        <v>20.86193084716797</v>
+        <v>21.14395141601562</v>
       </c>
       <c r="E44">
         <v>919.7985693233386</v>
       </c>
       <c r="F44">
-        <v>158.7233123779297</v>
+        <v>156.6062469482422</v>
       </c>
       <c r="G44">
         <v>3.234936644182395</v>
@@ -1671,7 +1671,7 @@
         <v>3.212140446956366</v>
       </c>
       <c r="I44">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1682,16 +1682,16 @@
         <v>43</v>
       </c>
       <c r="C45">
-        <v>158.6932060969682</v>
+        <v>142.8487049681554</v>
       </c>
       <c r="D45">
-        <v>41.64458084106445</v>
+        <v>40.56056976318359</v>
       </c>
       <c r="E45">
         <v>551.9324064875545</v>
       </c>
       <c r="F45">
-        <v>47.71224975585938</v>
+        <v>48.98739624023438</v>
       </c>
       <c r="G45">
         <v>-1.941400280353867</v>
@@ -1700,7 +1700,7 @@
         <v>8.736348125741674</v>
       </c>
       <c r="I45">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1711,16 +1711,16 @@
         <v>44</v>
       </c>
       <c r="C46">
-        <v>176.7011273711588</v>
+        <v>212.4454881299296</v>
       </c>
       <c r="D46">
-        <v>31.33520698547363</v>
+        <v>33.65685653686523</v>
       </c>
       <c r="E46">
         <v>207.6893822174316</v>
       </c>
       <c r="F46">
-        <v>23.86075592041016</v>
+        <v>22.21484184265137</v>
       </c>
       <c r="G46">
         <v>0.3983383409993186</v>
@@ -1729,7 +1729,7 @@
         <v>9.769148550392874</v>
       </c>
       <c r="I46">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1740,16 +1740,16 @@
         <v>45</v>
       </c>
       <c r="C47">
-        <v>156.3656535180437</v>
+        <v>155.4427681289725</v>
       </c>
       <c r="D47">
-        <v>42.51509857177734</v>
+        <v>42.47409439086914</v>
       </c>
       <c r="E47">
         <v>938.7045830726238</v>
       </c>
       <c r="F47">
-        <v>79.48556518554688</v>
+        <v>79.56229400634766</v>
       </c>
       <c r="G47">
         <v>-2.387654775159163</v>
@@ -1758,7 +1758,7 @@
         <v>3.048267834828779</v>
       </c>
       <c r="I47">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1769,16 +1769,16 @@
         <v>46</v>
       </c>
       <c r="C48">
-        <v>189.740701749735</v>
+        <v>174.5347071149532</v>
       </c>
       <c r="D48">
-        <v>32.98342514038086</v>
+        <v>31.97195625305176</v>
       </c>
       <c r="E48">
         <v>25.27869677441049</v>
       </c>
       <c r="F48">
-        <v>2.759061574935913</v>
+        <v>2.846347808837891</v>
       </c>
       <c r="G48">
         <v>0.2381323032010778</v>
@@ -1787,7 +1787,7 @@
         <v>9.671196658366</v>
       </c>
       <c r="I48">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1798,16 +1798,16 @@
         <v>47</v>
       </c>
       <c r="C49">
-        <v>159.5557684807409</v>
+        <v>140.8318539300991</v>
       </c>
       <c r="D49">
-        <v>42.88124084472656</v>
+        <v>42.04850769042969</v>
       </c>
       <c r="E49">
         <v>710.8830771958565</v>
       </c>
       <c r="F49">
-        <v>59.68061828613281</v>
+        <v>60.8625373840332</v>
       </c>
       <c r="G49">
         <v>-2.316807924352409</v>
@@ -1816,7 +1816,7 @@
         <v>6.329466394030306</v>
       </c>
       <c r="I49">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1827,16 +1827,16 @@
         <v>48</v>
       </c>
       <c r="C50">
-        <v>187.6193186265334</v>
+        <v>198.8946582703525</v>
       </c>
       <c r="D50">
-        <v>32.92135620117188</v>
+        <v>33.65182113647461</v>
       </c>
       <c r="E50">
         <v>13.61530962919642</v>
       </c>
       <c r="F50">
-        <v>1.488854646682739</v>
+        <v>1.456536650657654</v>
       </c>
       <c r="G50">
         <v>0.1923887149861216</v>
@@ -1845,7 +1845,7 @@
         <v>8.616249065587811</v>
       </c>
       <c r="I50">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1874,7 +1874,7 @@
         <v>9.478193265144439</v>
       </c>
       <c r="I51">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1885,16 +1885,16 @@
         <v>50</v>
       </c>
       <c r="C52">
-        <v>225.6925624474521</v>
+        <v>213.8520578460609</v>
       </c>
       <c r="D52">
-        <v>26.1749267578125</v>
+        <v>25.42654800415039</v>
       </c>
       <c r="E52">
         <v>435.5356769315731</v>
       </c>
       <c r="F52">
-        <v>59.90192413330078</v>
+        <v>61.66501235961914</v>
       </c>
       <c r="G52">
         <v>1.974519515110574</v>
@@ -1903,7 +1903,7 @@
         <v>6.773746381148227</v>
       </c>
       <c r="I52">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1914,16 +1914,16 @@
         <v>51</v>
       </c>
       <c r="C53">
-        <v>106.9720709986823</v>
+        <v>108.9966061880305</v>
       </c>
       <c r="D53">
-        <v>48.89583587646484</v>
+        <v>48.79267501831055</v>
       </c>
       <c r="E53">
         <v>1558.661065889315</v>
       </c>
       <c r="F53">
-        <v>114.7578201293945</v>
+        <v>115.0004501342773</v>
       </c>
       <c r="G53">
         <v>-4.645913252401428</v>
@@ -1932,7 +1932,7 @@
         <v>9.100209265993705</v>
       </c>
       <c r="I53">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -1943,16 +1943,16 @@
         <v>52</v>
       </c>
       <c r="C54">
-        <v>196.3067975683373</v>
+        <v>236.6257083510855</v>
       </c>
       <c r="D54">
-        <v>24.25494575500488</v>
+        <v>26.80330085754395</v>
       </c>
       <c r="E54">
         <v>755.2700581801146</v>
       </c>
       <c r="F54">
-        <v>112.0997085571289</v>
+        <v>101.4416885375977</v>
       </c>
       <c r="G54">
         <v>2.031562830371228</v>
@@ -1961,7 +1961,7 @@
         <v>8.803832620215976</v>
       </c>
       <c r="I54">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -1972,16 +1972,16 @@
         <v>53</v>
       </c>
       <c r="C55">
-        <v>150.5113301090585</v>
+        <v>146.1925760631464</v>
       </c>
       <c r="D55">
-        <v>43.53732299804688</v>
+        <v>43.34547424316406</v>
       </c>
       <c r="E55">
         <v>1264.899823143351</v>
       </c>
       <c r="F55">
-        <v>104.5916137695312</v>
+        <v>105.0545425415039</v>
       </c>
       <c r="G55">
         <v>-2.706180481819132</v>
@@ -1990,7 +1990,7 @@
         <v>2.715786035652243</v>
       </c>
       <c r="I55">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2001,16 +2001,16 @@
         <v>54</v>
       </c>
       <c r="C56">
-        <v>204.3318717681407</v>
+        <v>205.7392644122634</v>
       </c>
       <c r="D56">
-        <v>32.97794342041016</v>
+        <v>33.06689834594727</v>
       </c>
       <c r="E56">
         <v>12.47517702549885</v>
       </c>
       <c r="F56">
-        <v>1.361838579177856</v>
+        <v>1.358175039291382</v>
       </c>
       <c r="G56">
         <v>0.1809728507841649</v>
@@ -2019,7 +2019,7 @@
         <v>-0.9691183484051571</v>
       </c>
       <c r="I56">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2030,16 +2030,16 @@
         <v>55</v>
       </c>
       <c r="C57">
-        <v>199.4627026402702</v>
+        <v>202.1519566930756</v>
       </c>
       <c r="D57">
-        <v>34.32258605957031</v>
+        <v>34.49256134033203</v>
       </c>
       <c r="E57">
         <v>25.59575949009377</v>
       </c>
       <c r="F57">
-        <v>2.684667587280273</v>
+        <v>2.671437740325928</v>
       </c>
       <c r="G57">
         <v>-0.1671179263512283</v>
@@ -2048,7 +2048,7 @@
         <v>-1.836499198479489</v>
       </c>
       <c r="I57">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2059,16 +2059,16 @@
         <v>56</v>
       </c>
       <c r="C58">
-        <v>207.0759938260275</v>
+        <v>202.897288125262</v>
       </c>
       <c r="D58">
-        <v>33.49795532226562</v>
+        <v>33.23383712768555</v>
       </c>
       <c r="E58">
         <v>12.64423606528362</v>
       </c>
       <c r="F58">
-        <v>1.358866453170776</v>
+        <v>1.369665741920471</v>
       </c>
       <c r="G58">
         <v>0.0996391493335807</v>
@@ -2077,7 +2077,7 @@
         <v>-1.530310538753543</v>
       </c>
       <c r="I58">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2088,16 +2088,16 @@
         <v>57</v>
       </c>
       <c r="C59">
-        <v>202.2231268443722</v>
+        <v>200.8508955759284</v>
       </c>
       <c r="D59">
-        <v>33.80237197875977</v>
+        <v>33.71564102172852</v>
       </c>
       <c r="E59">
         <v>12.5971306548563</v>
       </c>
       <c r="F59">
-        <v>1.341611981391907</v>
+        <v>1.345063328742981</v>
       </c>
       <c r="G59">
         <v>-0.01533163524593177</v>
@@ -2106,7 +2106,7 @@
         <v>-1.223801256598705</v>
       </c>
       <c r="I59">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2117,16 +2117,16 @@
         <v>58</v>
       </c>
       <c r="C60">
-        <v>205.8077968839932</v>
+        <v>203.0468596901894</v>
       </c>
       <c r="D60">
-        <v>33.79060363769531</v>
+        <v>33.6161003112793</v>
       </c>
       <c r="E60">
         <v>23.20820445037316</v>
       </c>
       <c r="F60">
-        <v>2.472567081451416</v>
+        <v>2.485402345657349</v>
       </c>
       <c r="G60">
         <v>0.03034269269324871</v>
@@ -2135,7 +2135,7 @@
         <v>-1.305201694265891</v>
       </c>
       <c r="I60">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2146,16 +2146,16 @@
         <v>59</v>
       </c>
       <c r="C61">
-        <v>202.2166817268425</v>
+        <v>199.4995197124495</v>
       </c>
       <c r="D61">
-        <v>34.13421630859375</v>
+        <v>33.96247863769531</v>
       </c>
       <c r="E61">
         <v>34.456874764448</v>
       </c>
       <c r="F61">
-        <v>3.634029626846313</v>
+        <v>3.652405738830566</v>
       </c>
       <c r="G61">
         <v>-0.09062660158489143</v>
@@ -2164,7 +2164,7 @@
         <v>-1.639802592446514</v>
       </c>
       <c r="I61">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2175,16 +2175,16 @@
         <v>60</v>
       </c>
       <c r="C62">
-        <v>204.9883564185058</v>
+        <v>203.6023330876295</v>
       </c>
       <c r="D62">
-        <v>33.60673522949219</v>
+        <v>33.51913452148438</v>
       </c>
       <c r="E62">
         <v>41.78436304307252</v>
       </c>
       <c r="F62">
-        <v>4.475998878479004</v>
+        <v>4.487696170806885</v>
       </c>
       <c r="G62">
         <v>0.0612476728704989</v>
@@ -2193,7 +2193,7 @@
         <v>-1.095450470097568</v>
       </c>
       <c r="I62">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2204,16 +2204,16 @@
         <v>61</v>
       </c>
       <c r="C63">
-        <v>199.9168610493481</v>
+        <v>202.6424542018602</v>
       </c>
       <c r="D63">
-        <v>33.90943145751953</v>
+        <v>34.08169937133789</v>
       </c>
       <c r="E63">
         <v>21.47750869284573</v>
       </c>
       <c r="F63">
-        <v>2.280163049697876</v>
+        <v>2.268637657165527</v>
       </c>
       <c r="G63">
         <v>-0.06742437242755824</v>
@@ -2222,7 +2222,7 @@
         <v>-1.303367942610337</v>
       </c>
       <c r="I63">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2233,16 +2233,16 @@
         <v>62</v>
       </c>
       <c r="C64">
-        <v>213.2296123447653</v>
+        <v>210.3513674448669</v>
       </c>
       <c r="D64">
-        <v>32.41071319580078</v>
+        <v>32.22879028320312</v>
       </c>
       <c r="E64">
         <v>219.7798828132327</v>
       </c>
       <c r="F64">
-        <v>24.41191291809082</v>
+        <v>24.54971122741699</v>
       </c>
       <c r="G64">
         <v>0.3614021000029659</v>
@@ -2251,7 +2251,7 @@
         <v>-2.996890153055212</v>
       </c>
       <c r="I64">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -2262,16 +2262,16 @@
         <v>63</v>
       </c>
       <c r="C65">
-        <v>161.9518584640765</v>
+        <v>150.1490235206237</v>
       </c>
       <c r="D65">
-        <v>43.17078018188477</v>
+        <v>42.64833068847656</v>
       </c>
       <c r="E65">
         <v>570.7407078778269</v>
       </c>
       <c r="F65">
-        <v>47.59391784667969</v>
+        <v>48.17695236206055</v>
       </c>
       <c r="G65">
         <v>-2.819358949109247</v>
@@ -2280,7 +2280,7 @@
         <v>-4.047118092241034</v>
       </c>
       <c r="I65">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2291,16 +2291,16 @@
         <v>64</v>
       </c>
       <c r="C66">
-        <v>222.6789171192806</v>
+        <v>221.1021279480878</v>
       </c>
       <c r="D66">
-        <v>29.29891204833984</v>
+        <v>29.19924736022949</v>
       </c>
       <c r="E66">
         <v>1701.564347687097</v>
       </c>
       <c r="F66">
-        <v>209.0736846923828</v>
+        <v>209.7873229980469</v>
       </c>
       <c r="G66">
         <v>1.192672554068895</v>
@@ -2309,7 +2309,7 @@
         <v>1.224496329143648</v>
       </c>
       <c r="I66">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2320,16 +2320,16 @@
         <v>65</v>
       </c>
       <c r="C67">
-        <v>159.2816214104639</v>
+        <v>158.3388051963592</v>
       </c>
       <c r="D67">
-        <v>41.8033561706543</v>
+        <v>41.761474609375</v>
       </c>
       <c r="E67">
         <v>1238.094529523736</v>
       </c>
       <c r="F67">
-        <v>106.6215896606445</v>
+        <v>106.728515625</v>
       </c>
       <c r="G67">
         <v>-2.281667608214841</v>
@@ -2338,7 +2338,7 @@
         <v>0.5497540025124052</v>
       </c>
       <c r="I67">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2349,16 +2349,16 @@
         <v>66</v>
       </c>
       <c r="C68">
-        <v>248.4270775001456</v>
+        <v>252.1704872450465</v>
       </c>
       <c r="D68">
-        <v>19.86155891418457</v>
+        <v>20.06499862670898</v>
       </c>
       <c r="E68">
         <v>1478.37646889903</v>
       </c>
       <c r="F68">
-        <v>267.9626159667969</v>
+        <v>265.2457275390625</v>
       </c>
       <c r="G68">
         <v>3.513903955135374</v>
@@ -2367,7 +2367,7 @@
         <v>1.309943888990366</v>
       </c>
       <c r="I68">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2378,16 +2378,16 @@
         <v>67</v>
       </c>
       <c r="C69">
-        <v>206.677662408864</v>
+        <v>193.4704226927835</v>
       </c>
       <c r="D69">
-        <v>37.88132095336914</v>
+        <v>37.15493774414062</v>
       </c>
       <c r="E69">
         <v>292.6010743627921</v>
       </c>
       <c r="F69">
-        <v>27.80694580078125</v>
+        <v>28.35057640075684</v>
       </c>
       <c r="G69">
         <v>-0.9351353751330883</v>
@@ -2396,7 +2396,7 @@
         <v>-4.295350749098601</v>
       </c>
       <c r="I69">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2407,16 +2407,16 @@
         <v>68</v>
       </c>
       <c r="C70">
-        <v>204.0889081854114</v>
+        <v>202.6980191035573</v>
       </c>
       <c r="D70">
-        <v>33.49015426635742</v>
+        <v>33.40224456787109</v>
       </c>
       <c r="E70">
         <v>20.36903480348701</v>
       </c>
       <c r="F70">
-        <v>2.189554691314697</v>
+        <v>2.195317268371582</v>
       </c>
       <c r="G70">
         <v>0.08839089202534364</v>
@@ -2425,7 +2425,7 @@
         <v>-0.4008727633516296</v>
       </c>
       <c r="I70">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -2436,16 +2436,16 @@
         <v>69</v>
       </c>
       <c r="C71">
-        <v>193.9561153807263</v>
+        <v>200.469050500965</v>
       </c>
       <c r="D71">
-        <v>35.09585952758789</v>
+        <v>35.50751113891602</v>
       </c>
       <c r="E71">
         <v>18.65366707263456</v>
       </c>
       <c r="F71">
-        <v>1.913422346115112</v>
+        <v>1.891239404678345</v>
       </c>
       <c r="G71">
         <v>-0.3949548349024165</v>
@@ -2454,7 +2454,7 @@
         <v>-2.043470506630904</v>
       </c>
       <c r="I71">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -2465,16 +2465,16 @@
         <v>70</v>
       </c>
       <c r="C72">
-        <v>249.4013982324924</v>
+        <v>251.2271546506359</v>
       </c>
       <c r="D72">
-        <v>21.76424407958984</v>
+        <v>21.86346626281738</v>
       </c>
       <c r="E72">
         <v>1192.852900399776</v>
       </c>
       <c r="F72">
-        <v>197.3085021972656</v>
+        <v>196.4130554199219</v>
       </c>
       <c r="G72">
         <v>3.068620452199015</v>
@@ -2483,7 +2483,7 @@
         <v>-1.802040962007777</v>
       </c>
       <c r="I72">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -2494,16 +2494,16 @@
         <v>71</v>
       </c>
       <c r="C73">
-        <v>200.7684748740211</v>
+        <v>199.4107901252809</v>
       </c>
       <c r="D73">
-        <v>34.05614852905273</v>
+        <v>33.9703369140625</v>
       </c>
       <c r="E73">
         <v>39.58186892988306</v>
       </c>
       <c r="F73">
-        <v>4.184111595153809</v>
+        <v>4.194680690765381</v>
       </c>
       <c r="G73">
         <v>-0.09555382349409856</v>
@@ -2512,7 +2512,7 @@
         <v>-1.742113006776057</v>
       </c>
       <c r="I73">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -2523,16 +2523,16 @@
         <v>72</v>
       </c>
       <c r="C74">
-        <v>206.1993573721452</v>
+        <v>207.6256135072174</v>
       </c>
       <c r="D74">
-        <v>32.49396896362305</v>
+        <v>32.58411026000977</v>
       </c>
       <c r="E74">
         <v>89.59064185099123</v>
       </c>
       <c r="F74">
-        <v>9.925727844238281</v>
+        <v>9.898269653320312</v>
       </c>
       <c r="G74">
         <v>0.2878333828145256</v>
@@ -2541,7 +2541,7 @@
         <v>-1.56225071611269</v>
       </c>
       <c r="I74">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -2552,16 +2552,16 @@
         <v>73</v>
       </c>
       <c r="C75">
-        <v>191.6460152902696</v>
+        <v>194.2306278472139</v>
       </c>
       <c r="D75">
-        <v>35.08139038085938</v>
+        <v>35.24475479125977</v>
       </c>
       <c r="E75">
         <v>113.1510649064658</v>
       </c>
       <c r="F75">
-        <v>11.61139297485352</v>
+        <v>11.55757236480713</v>
       </c>
       <c r="G75">
         <v>-0.4501397728075357</v>
@@ -2570,7 +2570,7 @@
         <v>-3.364038488402069</v>
       </c>
       <c r="I75">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -2581,16 +2581,16 @@
         <v>74</v>
       </c>
       <c r="C76">
-        <v>207.0760925778285</v>
+        <v>205.6967130382379</v>
       </c>
       <c r="D76">
-        <v>33.73080444335938</v>
+        <v>33.64362335205078</v>
       </c>
       <c r="E76">
         <v>35.79399999910675</v>
       </c>
       <c r="F76">
-        <v>3.820199251174927</v>
+        <v>3.830098390579224</v>
       </c>
       <c r="G76">
         <v>0.02429351747549238</v>
@@ -2599,7 +2599,7 @@
         <v>-2.850329613276325</v>
       </c>
       <c r="I76">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -2610,16 +2610,16 @@
         <v>75</v>
       </c>
       <c r="C77">
-        <v>211.5045572426403</v>
+        <v>203.6259581097222</v>
       </c>
       <c r="D77">
-        <v>36.98584365844727</v>
+        <v>36.55760955810547</v>
       </c>
       <c r="E77">
         <v>122.4589308720097</v>
       </c>
       <c r="F77">
-        <v>11.91948318481445</v>
+        <v>12.05910682678223</v>
       </c>
       <c r="G77">
         <v>-0.6813108349116376</v>
@@ -2628,7 +2628,7 @@
         <v>-4.546921201111702</v>
       </c>
       <c r="I77">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -2657,7 +2657,7 @@
         <v>-0.7150572444261751</v>
       </c>
       <c r="I78">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -2668,16 +2668,16 @@
         <v>77</v>
       </c>
       <c r="C79">
-        <v>199.0121265846156</v>
+        <v>197.6720053187694</v>
       </c>
       <c r="D79">
-        <v>34.68062973022461</v>
+        <v>34.59592819213867</v>
       </c>
       <c r="E79">
         <v>74.4020240477912</v>
       </c>
       <c r="F79">
-        <v>7.723252773284912</v>
+        <v>7.742161750793457</v>
       </c>
       <c r="G79">
         <v>-0.191718887208056</v>
@@ -2686,7 +2686,7 @@
         <v>0.5490306867231698</v>
       </c>
       <c r="I79">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -2697,16 +2697,16 @@
         <v>78</v>
       </c>
       <c r="C80">
-        <v>206.9435827365307</v>
+        <v>208.377356299526</v>
       </c>
       <c r="D80">
-        <v>32.50057983398438</v>
+        <v>32.5911979675293</v>
       </c>
       <c r="E80">
         <v>21.65612692477589</v>
       </c>
       <c r="F80">
-        <v>2.398789644241333</v>
+        <v>2.392119884490967</v>
       </c>
       <c r="G80">
         <v>0.330747838116172</v>
@@ -2715,7 +2715,7 @@
         <v>0.02587660591580461</v>
       </c>
       <c r="I80">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -2726,16 +2726,16 @@
         <v>79</v>
       </c>
       <c r="C81">
-        <v>205.0205549350627</v>
+        <v>206.3669064248229</v>
       </c>
       <c r="D81">
-        <v>34.35954284667969</v>
+        <v>34.44419097900391</v>
       </c>
       <c r="E81">
         <v>75.08637616922351</v>
       </c>
       <c r="F81">
-        <v>7.867128849029541</v>
+        <v>7.847794532775879</v>
       </c>
       <c r="G81">
         <v>-0.1576901133683288</v>
@@ -2744,7 +2744,7 @@
         <v>-4.258154043925821</v>
       </c>
       <c r="I81">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -2755,16 +2755,16 @@
         <v>80</v>
       </c>
       <c r="C82">
-        <v>234.251144803779</v>
+        <v>235.9607523270495</v>
       </c>
       <c r="D82">
-        <v>25.37860107421875</v>
+        <v>25.48665428161621</v>
       </c>
       <c r="E82">
         <v>2427.044252905944</v>
       </c>
       <c r="F82">
-        <v>344.2805480957031</v>
+        <v>342.8209228515625</v>
       </c>
       <c r="G82">
         <v>2.10853553547893</v>
@@ -2773,7 +2773,7 @@
         <v>0.7481270099782461</v>
       </c>
       <c r="I82">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -2784,16 +2784,16 @@
         <v>81</v>
       </c>
       <c r="C83">
-        <v>153.1169530611619</v>
+        <v>145.9237324031079</v>
       </c>
       <c r="D83">
-        <v>42.90610885620117</v>
+        <v>42.58656311035156</v>
       </c>
       <c r="E83">
         <v>3454.663685947395</v>
       </c>
       <c r="F83">
-        <v>289.8605651855469</v>
+        <v>292.0354919433594</v>
       </c>
       <c r="G83">
         <v>-2.514697343303455</v>
@@ -2802,7 +2802,7 @@
         <v>3.065985608365474</v>
       </c>
       <c r="I83">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -2813,16 +2813,16 @@
         <v>82</v>
       </c>
       <c r="C84">
-        <v>243.8586712980988</v>
+        <v>230.3599036529592</v>
       </c>
       <c r="D84">
-        <v>26.51916694641113</v>
+        <v>25.66887855529785</v>
       </c>
       <c r="E84">
         <v>490.2055269807897</v>
       </c>
       <c r="F84">
-        <v>66.54582214355469</v>
+        <v>68.75017547607422</v>
       </c>
       <c r="G84">
         <v>1.944243625895261</v>
@@ -2831,7 +2831,7 @@
         <v>-2.419328873481414</v>
       </c>
       <c r="I84">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -2842,16 +2842,16 @@
         <v>83</v>
       </c>
       <c r="C85">
-        <v>180.667080300096</v>
+        <v>177.2981362136854</v>
       </c>
       <c r="D85">
-        <v>37.80968475341797</v>
+        <v>37.62138366699219</v>
       </c>
       <c r="E85">
         <v>527.239657418635</v>
       </c>
       <c r="F85">
-        <v>50.200439453125</v>
+        <v>50.45169830322266</v>
       </c>
       <c r="G85">
         <v>-1.340100708621075</v>
@@ -2860,7 +2860,7 @@
         <v>-5.772312393461049</v>
       </c>
       <c r="I85">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se añaden comentarios y se simplifica el código
</commit_message>
<xml_diff>
--- a/Simulador/res_sim.xlsx
+++ b/Simulador/res_sim.xlsx
@@ -435,16 +435,16 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>212.4100882852489</v>
+        <v>214.047978155085</v>
       </c>
       <c r="D2">
-        <v>26.8738899230957</v>
+        <v>26.97741508483887</v>
       </c>
       <c r="E2">
         <v>344.0415503671599</v>
       </c>
       <c r="F2">
-        <v>46.08747100830078</v>
+        <v>45.91061019897461</v>
       </c>
       <c r="G2">
         <v>1.596116034322399</v>
@@ -453,7 +453,7 @@
         <v>3.492272793926644</v>
       </c>
       <c r="I2">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -464,16 +464,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>195.8442626255413</v>
+        <v>198.5145536995319</v>
       </c>
       <c r="D3">
-        <v>34.72961807250977</v>
+        <v>34.89839172363281</v>
       </c>
       <c r="E3">
         <v>13.56729663011254</v>
       </c>
       <c r="F3">
-        <v>1.406357765197754</v>
+        <v>1.399556398391724</v>
       </c>
       <c r="G3">
         <v>-0.2188322408916709</v>
@@ -482,7 +482,7 @@
         <v>1.57454844203958</v>
       </c>
       <c r="I3">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -493,16 +493,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>207.6413092108305</v>
+        <v>204.7596666005107</v>
       </c>
       <c r="D4">
-        <v>32.52976226806641</v>
+        <v>32.34762954711914</v>
       </c>
       <c r="E4">
         <v>168.9935131340457</v>
       </c>
       <c r="F4">
-        <v>18.7021541595459</v>
+        <v>18.80745697021484</v>
       </c>
       <c r="G4">
         <v>0.3711593507547151</v>
@@ -511,7 +511,7 @@
         <v>1.731397461341183</v>
       </c>
       <c r="I4">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -522,16 +522,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>199.9137848257901</v>
+        <v>198.5510193224993</v>
       </c>
       <c r="D5">
-        <v>34.22743606567383</v>
+        <v>34.14130401611328</v>
       </c>
       <c r="E5">
         <v>17.33180625774378</v>
       </c>
       <c r="F5">
-        <v>1.822938084602356</v>
+        <v>1.827537059783936</v>
       </c>
       <c r="G5">
         <v>-0.0675955599860016</v>
@@ -540,7 +540,7 @@
         <v>1.57520843538257</v>
       </c>
       <c r="I5">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -551,16 +551,16 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>195.5036422877196</v>
+        <v>196.8919789078017</v>
       </c>
       <c r="D6">
-        <v>33.43892669677734</v>
+        <v>33.52667999267578</v>
       </c>
       <c r="E6">
         <v>48.49833201473393</v>
       </c>
       <c r="F6">
-        <v>5.221279621124268</v>
+        <v>5.207613468170166</v>
       </c>
       <c r="G6">
         <v>0.07414374889212304</v>
@@ -569,7 +569,7 @@
         <v>3.40763809526817</v>
       </c>
       <c r="I6">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -580,16 +580,16 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>199.4536733531874</v>
+        <v>189.8498395422455</v>
       </c>
       <c r="D7">
-        <v>34.08193588256836</v>
+        <v>33.47492218017578</v>
       </c>
       <c r="E7">
         <v>15.03489657772798</v>
       </c>
       <c r="F7">
-        <v>1.588103055953979</v>
+        <v>1.61690080165863</v>
       </c>
       <c r="G7">
         <v>-0.01674270518462065</v>
@@ -598,7 +598,7 @@
         <v>2.835582102804634</v>
       </c>
       <c r="I7">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -609,16 +609,16 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>196.985950004047</v>
+        <v>189.8899311866251</v>
       </c>
       <c r="D8">
-        <v>32.80995559692383</v>
+        <v>32.3614501953125</v>
       </c>
       <c r="E8">
         <v>55.21180257348544</v>
       </c>
       <c r="F8">
-        <v>6.057993412017822</v>
+        <v>6.141952514648438</v>
       </c>
       <c r="G8">
         <v>0.2477469273428186</v>
@@ -627,7 +627,7 @@
         <v>4.760357197651417</v>
       </c>
       <c r="I8">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -638,16 +638,16 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>149.9973501570169</v>
+        <v>153.6531501637703</v>
       </c>
       <c r="D9">
-        <v>42.5806770324707</v>
+        <v>42.74308013916016</v>
       </c>
       <c r="E9">
         <v>560.0692098765884</v>
       </c>
       <c r="F9">
-        <v>47.35127258300781</v>
+        <v>47.17135620117188</v>
       </c>
       <c r="G9">
         <v>-2.435372970096637</v>
@@ -656,7 +656,7 @@
         <v>3.98256430003651</v>
       </c>
       <c r="I9">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -667,16 +667,16 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>249.5719941049813</v>
+        <v>244.3765521422868</v>
       </c>
       <c r="D10">
-        <v>24.86376190185547</v>
+        <v>24.53827667236328</v>
       </c>
       <c r="E10">
         <v>1382.447533600548</v>
       </c>
       <c r="F10">
-        <v>200.1632385253906</v>
+        <v>202.8182678222656</v>
       </c>
       <c r="G10">
         <v>2.353631628237696</v>
@@ -685,7 +685,7 @@
         <v>-3.902847856084686</v>
       </c>
       <c r="I10">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -696,16 +696,16 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>214.2764706860224</v>
+        <v>211.5868045475355</v>
       </c>
       <c r="D11">
-        <v>35.08147430419922</v>
+        <v>34.91147232055664</v>
       </c>
       <c r="E11">
         <v>199.1265320145867</v>
       </c>
       <c r="F11">
-        <v>20.43401908874512</v>
+        <v>20.53352165222168</v>
       </c>
       <c r="G11">
         <v>-0.1659918344285073</v>
@@ -714,7 +714,7 @@
         <v>-3.39453113286161</v>
       </c>
       <c r="I11">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -725,16 +725,16 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>208.3492898518012</v>
+        <v>205.5106900527556</v>
       </c>
       <c r="D12">
-        <v>32.69679260253906</v>
+        <v>32.51737976074219</v>
       </c>
       <c r="E12">
         <v>91.86067101041317</v>
       </c>
       <c r="F12">
-        <v>10.11409378051758</v>
+        <v>10.16989707946777</v>
       </c>
       <c r="G12">
         <v>0.2482922711943954</v>
@@ -743,7 +743,7 @@
         <v>-2.756201684925812</v>
       </c>
       <c r="I12">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -754,16 +754,16 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>198.0122294824504</v>
+        <v>196.6821071876259</v>
       </c>
       <c r="D13">
-        <v>34.76255798339844</v>
+        <v>34.67848587036133</v>
       </c>
       <c r="E13">
         <v>13.58046852523921</v>
       </c>
       <c r="F13">
-        <v>1.406389117240906</v>
+        <v>1.409798741340637</v>
       </c>
       <c r="G13">
         <v>-0.2461488251019247</v>
@@ -772,7 +772,7 @@
         <v>-0.6139341684454964</v>
       </c>
       <c r="I13">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -783,16 +783,16 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>248.3795926524217</v>
+        <v>250.2319117701229</v>
       </c>
       <c r="D14">
-        <v>20.65255737304688</v>
+        <v>20.75322341918945</v>
       </c>
       <c r="E14">
         <v>1755.103346009126</v>
       </c>
       <c r="F14">
-        <v>305.9365539550781</v>
+        <v>304.4525756835938</v>
       </c>
       <c r="G14">
         <v>3.32023723483058</v>
@@ -801,7 +801,7 @@
         <v>-2.486692203613646</v>
       </c>
       <c r="I14">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -812,16 +812,16 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>220.4471407469995</v>
+        <v>213.7424961831204</v>
       </c>
       <c r="D15">
-        <v>34.64437484741211</v>
+        <v>34.22924423217773</v>
       </c>
       <c r="E15">
         <v>26.87268222576495</v>
       </c>
       <c r="F15">
-        <v>2.792420148849487</v>
+        <v>2.826286792755127</v>
       </c>
       <c r="G15">
         <v>-0.05742926703369799</v>
@@ -830,7 +830,7 @@
         <v>-4.904003908876237</v>
       </c>
       <c r="I15">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -841,16 +841,16 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>222.7108238046733</v>
+        <v>221.1173352086559</v>
       </c>
       <c r="D16">
-        <v>33.77034759521484</v>
+        <v>33.673828125</v>
       </c>
       <c r="E16">
         <v>18.32142955760628</v>
       </c>
       <c r="F16">
-        <v>1.953108310699463</v>
+        <v>1.958706498146057</v>
       </c>
       <c r="G16">
         <v>0.1052479458827658</v>
@@ -859,7 +859,7 @@
         <v>-5.685938728369462</v>
       </c>
       <c r="I16">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -870,16 +870,16 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>160.8404833792993</v>
+        <v>177.5893057174293</v>
       </c>
       <c r="D17">
-        <v>40.97915649414062</v>
+        <v>41.86480331420898</v>
       </c>
       <c r="E17">
         <v>778.6626264767738</v>
       </c>
       <c r="F17">
-        <v>68.40514373779297</v>
+        <v>66.95804595947266</v>
       </c>
       <c r="G17">
         <v>-2.347143802750921</v>
@@ -888,7 +888,7 @@
         <v>-5.184267536920604</v>
       </c>
       <c r="I17">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -899,16 +899,16 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>209.414647058288</v>
+        <v>210.8733808669576</v>
       </c>
       <c r="D18">
-        <v>31.7907772064209</v>
+        <v>31.88297653198242</v>
       </c>
       <c r="E18">
         <v>118.2246671331604</v>
       </c>
       <c r="F18">
-        <v>13.38780784606934</v>
+        <v>13.34909248352051</v>
       </c>
       <c r="G18">
         <v>0.4746819056162278</v>
@@ -917,7 +917,7 @@
         <v>-1.272944327177375</v>
       </c>
       <c r="I18">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -928,16 +928,16 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>173.2397206866067</v>
+        <v>159.1214962492232</v>
       </c>
       <c r="D19">
-        <v>41.46060562133789</v>
+        <v>40.7130012512207</v>
       </c>
       <c r="E19">
         <v>2858.371279980439</v>
       </c>
       <c r="F19">
-        <v>248.1906890869141</v>
+        <v>252.7481842041016</v>
       </c>
       <c r="G19">
         <v>-2.290160995983005</v>
@@ -946,7 +946,7 @@
         <v>-4.949172023586057</v>
       </c>
       <c r="I19">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -957,16 +957,16 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>225.6592358795646</v>
+        <v>202.4778271633178</v>
       </c>
       <c r="D20">
-        <v>31.68818473815918</v>
+        <v>30.23079490661621</v>
       </c>
       <c r="E20">
         <v>102.3123986075007</v>
       </c>
       <c r="F20">
-        <v>11.62340545654297</v>
+        <v>12.18375682830811</v>
       </c>
       <c r="G20">
         <v>0.3209526194120306</v>
@@ -975,7 +975,7 @@
         <v>-9.70486363213517</v>
       </c>
       <c r="I20">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -986,16 +986,16 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>194.1141376542186</v>
+        <v>218.9270994375812</v>
       </c>
       <c r="D21">
-        <v>31.98231506347656</v>
+        <v>33.54227447509766</v>
       </c>
       <c r="E21">
         <v>30.59651750363264</v>
       </c>
       <c r="F21">
-        <v>3.444011449813843</v>
+        <v>3.28383994102478</v>
       </c>
       <c r="G21">
         <v>-0.1654132108420091</v>
@@ -1004,7 +1004,7 @@
         <v>-9.861219867994032</v>
       </c>
       <c r="I21">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1015,16 +1015,16 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>204.2063978483665</v>
+        <v>221.5035447084712</v>
       </c>
       <c r="D22">
-        <v>31.91837120056152</v>
+        <v>33.00582122802734</v>
       </c>
       <c r="E22">
         <v>24.03705720769904</v>
       </c>
       <c r="F22">
-        <v>2.711084604263306</v>
+        <v>2.621762037277222</v>
       </c>
       <c r="G22">
         <v>0.01819589233524954</v>
@@ -1033,7 +1033,7 @@
         <v>-9.279345091961993</v>
       </c>
       <c r="I22">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1062,7 +1062,7 @@
         <v>-9.238281327998019</v>
       </c>
       <c r="I23">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1091,7 +1091,7 @@
         <v>-9.954147471937697</v>
       </c>
       <c r="I24">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1120,7 +1120,7 @@
         <v>-9.022411740833657</v>
       </c>
       <c r="I25">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1149,7 +1149,7 @@
         <v>-8.465904839481219</v>
       </c>
       <c r="I26">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1178,7 +1178,7 @@
         <v>-9.450384387180872</v>
       </c>
       <c r="I27">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1207,7 +1207,7 @@
         <v>-9.945059851748946</v>
       </c>
       <c r="I28">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1218,16 +1218,16 @@
         <v>27</v>
       </c>
       <c r="C29">
-        <v>219.8015722052845</v>
+        <v>195.2005414691534</v>
       </c>
       <c r="D29">
-        <v>33.44755554199219</v>
+        <v>31.90091896057129</v>
       </c>
       <c r="E29">
         <v>12.15827774819991</v>
       </c>
       <c r="F29">
-        <v>1.3086097240448</v>
+        <v>1.37205445766449</v>
       </c>
       <c r="G29">
         <v>-0.1034063002761221</v>
@@ -1236,7 +1236,7 @@
         <v>-9.385389381431935</v>
       </c>
       <c r="I29">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1265,7 +1265,7 @@
         <v>-6.42479720367449</v>
       </c>
       <c r="I30">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1276,16 +1276,16 @@
         <v>29</v>
       </c>
       <c r="C31">
-        <v>135.0613780158662</v>
+        <v>129.6720412454149</v>
       </c>
       <c r="D31">
-        <v>45.25009918212891</v>
+        <v>45.01069259643555</v>
       </c>
       <c r="E31">
         <v>561.0455563968753</v>
       </c>
       <c r="F31">
-        <v>44.63556671142578</v>
+        <v>44.87297821044922</v>
       </c>
       <c r="G31">
         <v>-3.228726121143762</v>
@@ -1294,7 +1294,7 @@
         <v>4.029840037148754</v>
       </c>
       <c r="I31">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1305,16 +1305,16 @@
         <v>30</v>
       </c>
       <c r="C32">
-        <v>178.8324503300365</v>
+        <v>210.8394569522468</v>
       </c>
       <c r="D32">
-        <v>30.38631439208984</v>
+        <v>32.40931701660156</v>
       </c>
       <c r="E32">
         <v>104.9411033259221</v>
       </c>
       <c r="F32">
-        <v>12.43283176422119</v>
+        <v>11.65676975250244</v>
       </c>
       <c r="G32">
         <v>0.5587509355297379</v>
@@ -1323,7 +1323,7 @@
         <v>7.35038777279619</v>
       </c>
       <c r="I32">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1334,16 +1334,16 @@
         <v>31</v>
       </c>
       <c r="C33">
-        <v>156.7458517647452</v>
+        <v>165.171491212528</v>
       </c>
       <c r="D33">
-        <v>41.15621948242188</v>
+        <v>41.56807327270508</v>
       </c>
       <c r="E33">
         <v>442.239946164329</v>
       </c>
       <c r="F33">
-        <v>38.68343353271484</v>
+        <v>38.3001594543457</v>
       </c>
       <c r="G33">
         <v>-2.31687999893804</v>
@@ -1352,7 +1352,7 @@
         <v>-2.995590014584259</v>
       </c>
       <c r="I33">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1363,16 +1363,16 @@
         <v>32</v>
       </c>
       <c r="C34">
-        <v>251.816684398179</v>
+        <v>249.9296471820358</v>
       </c>
       <c r="D34">
-        <v>19.37777900695801</v>
+        <v>19.27522468566895</v>
       </c>
       <c r="E34">
         <v>803.8684356637259</v>
       </c>
       <c r="F34">
-        <v>149.3425140380859</v>
+        <v>150.1370849609375</v>
       </c>
       <c r="G34">
         <v>3.67386674782785</v>
@@ -1381,7 +1381,7 @@
         <v>1.64528195886503</v>
       </c>
       <c r="I34">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1392,16 +1392,16 @@
         <v>33</v>
       </c>
       <c r="C35">
-        <v>179.7118444259558</v>
+        <v>178.5647259816962</v>
       </c>
       <c r="D35">
-        <v>38.32610702514648</v>
+        <v>38.26173782348633</v>
       </c>
       <c r="E35">
         <v>225.0946341554045</v>
       </c>
       <c r="F35">
-        <v>21.14330673217773</v>
+        <v>21.17887878417969</v>
       </c>
       <c r="G35">
         <v>-1.214580773440048</v>
@@ -1410,7 +1410,7 @@
         <v>0.03624061437360713</v>
       </c>
       <c r="I35">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1421,16 +1421,16 @@
         <v>34</v>
       </c>
       <c r="C36">
-        <v>253.2272975717206</v>
+        <v>255.1095705474378</v>
       </c>
       <c r="D36">
-        <v>19.65225410461426</v>
+        <v>19.75454711914062</v>
       </c>
       <c r="E36">
         <v>1544.238605138566</v>
       </c>
       <c r="F36">
-        <v>282.8815002441406</v>
+        <v>281.4166870117188</v>
       </c>
       <c r="G36">
         <v>3.623477518515383</v>
@@ -1439,7 +1439,7 @@
         <v>-1.280216372607037</v>
       </c>
       <c r="I36">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1450,16 +1450,16 @@
         <v>35</v>
       </c>
       <c r="C37">
-        <v>158.2100472575905</v>
+        <v>155.4137458398628</v>
       </c>
       <c r="D37">
-        <v>42.13228607177734</v>
+        <v>42.00806427001953</v>
       </c>
       <c r="E37">
         <v>916.9238501302698</v>
       </c>
       <c r="F37">
-        <v>78.34670257568359</v>
+        <v>78.57837677001953</v>
       </c>
       <c r="G37">
         <v>-2.338576875737777</v>
@@ -1468,7 +1468,7 @@
         <v>1.418178375911533</v>
       </c>
       <c r="I37">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1479,16 +1479,16 @@
         <v>36</v>
       </c>
       <c r="C38">
-        <v>221.9048797289773</v>
+        <v>197.8135917574117</v>
       </c>
       <c r="D38">
-        <v>33.74606323242188</v>
+        <v>32.23442077636719</v>
       </c>
       <c r="E38">
         <v>30.13365751333913</v>
       </c>
       <c r="F38">
-        <v>3.2146315574646</v>
+        <v>3.365382671356201</v>
       </c>
       <c r="G38">
         <v>0.04705830724490476</v>
@@ -1497,7 +1497,7 @@
         <v>-6.504653418974739</v>
       </c>
       <c r="I38">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1508,16 +1508,16 @@
         <v>37</v>
       </c>
       <c r="C39">
-        <v>192.7980056386309</v>
+        <v>194.0759856950172</v>
       </c>
       <c r="D39">
-        <v>35.30751037597656</v>
+        <v>35.38785552978516</v>
       </c>
       <c r="E39">
         <v>46.67657954138122</v>
       </c>
       <c r="F39">
-        <v>4.759204864501953</v>
+        <v>4.74839973449707</v>
       </c>
       <c r="G39">
         <v>-0.5267327097768739</v>
@@ -1526,7 +1526,7 @@
         <v>-4.414407877173214</v>
       </c>
       <c r="I39">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1537,16 +1537,16 @@
         <v>38</v>
       </c>
       <c r="C40">
-        <v>221.3879857072862</v>
+        <v>226.5436335877462</v>
       </c>
       <c r="D40">
-        <v>24.53653144836426</v>
+        <v>24.86239433288574</v>
       </c>
       <c r="E40">
         <v>1452.278941769579</v>
       </c>
       <c r="F40">
-        <v>213.078369140625</v>
+        <v>210.2856140136719</v>
       </c>
       <c r="G40">
         <v>2.176018014218581</v>
@@ -1555,7 +1555,7 @@
         <v>3.558546856154219</v>
       </c>
       <c r="I40">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1566,16 +1566,16 @@
         <v>39</v>
       </c>
       <c r="C41">
-        <v>194.073620314031</v>
+        <v>196.7077758306439</v>
       </c>
       <c r="D41">
-        <v>35.06266403198242</v>
+        <v>35.22916030883789</v>
       </c>
       <c r="E41">
         <v>340.4292798588431</v>
       </c>
       <c r="F41">
-        <v>34.9530029296875</v>
+        <v>34.78781127929688</v>
       </c>
       <c r="G41">
         <v>-0.3168343342728075</v>
@@ -1584,7 +1584,7 @@
         <v>1.146574443400988</v>
       </c>
       <c r="I41">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1613,7 +1613,7 @@
         <v>9.997376345115907</v>
       </c>
       <c r="I42">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1624,16 +1624,16 @@
         <v>41</v>
       </c>
       <c r="C43">
-        <v>170.1119185630267</v>
+        <v>171.1012072083258</v>
       </c>
       <c r="D43">
-        <v>33.19799423217773</v>
+        <v>33.26494598388672</v>
       </c>
       <c r="E43">
         <v>17.19116230919826</v>
       </c>
       <c r="F43">
-        <v>1.864214420318604</v>
+        <v>1.860462427139282</v>
       </c>
       <c r="G43">
         <v>-0.08132546284821182</v>
@@ -1642,7 +1642,7 @@
         <v>9.135520449007458</v>
       </c>
       <c r="I43">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1653,16 +1653,16 @@
         <v>42</v>
       </c>
       <c r="C44">
-        <v>247.5055084025498</v>
+        <v>245.6620184186856</v>
       </c>
       <c r="D44">
-        <v>21.0499439239502</v>
+        <v>20.9559383392334</v>
       </c>
       <c r="E44">
         <v>919.7985693233386</v>
       </c>
       <c r="F44">
-        <v>157.3056488037109</v>
+        <v>158.0112915039062</v>
       </c>
       <c r="G44">
         <v>3.234936644182395</v>
@@ -1671,7 +1671,7 @@
         <v>3.212140446956366</v>
       </c>
       <c r="I44">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1682,16 +1682,16 @@
         <v>43</v>
       </c>
       <c r="C45">
-        <v>161.7155675839672</v>
+        <v>142.8487049681554</v>
       </c>
       <c r="D45">
-        <v>41.80600738525391</v>
+        <v>40.56056976318359</v>
       </c>
       <c r="E45">
         <v>551.9324064875545</v>
       </c>
       <c r="F45">
-        <v>47.52801895141602</v>
+        <v>48.98739624023438</v>
       </c>
       <c r="G45">
         <v>-1.941400280353867</v>
@@ -1700,7 +1700,7 @@
         <v>8.736348125741674</v>
       </c>
       <c r="I45">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1711,16 +1711,16 @@
         <v>44</v>
       </c>
       <c r="C46">
-        <v>176.7011273711588</v>
+        <v>193.65341611337</v>
       </c>
       <c r="D46">
-        <v>31.33520698547363</v>
+        <v>32.43943023681641</v>
       </c>
       <c r="E46">
         <v>207.6893822174316</v>
       </c>
       <c r="F46">
-        <v>23.86075592041016</v>
+        <v>23.04854774475098</v>
       </c>
       <c r="G46">
         <v>0.3983383409993186</v>
@@ -1729,7 +1729,7 @@
         <v>9.769148550392874</v>
       </c>
       <c r="I46">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1740,16 +1740,16 @@
         <v>45</v>
       </c>
       <c r="C47">
-        <v>157.2885389071149</v>
+        <v>154.5198827399014</v>
       </c>
       <c r="D47">
-        <v>42.55609512329102</v>
+        <v>42.4330940246582</v>
       </c>
       <c r="E47">
         <v>938.7045830726238</v>
       </c>
       <c r="F47">
-        <v>79.40898895263672</v>
+        <v>79.63916778564453</v>
       </c>
       <c r="G47">
         <v>-2.387654775159163</v>
@@ -1758,7 +1758,7 @@
         <v>3.048267834828779</v>
       </c>
       <c r="I47">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1769,16 +1769,16 @@
         <v>46</v>
       </c>
       <c r="C48">
-        <v>174.5347071149532</v>
+        <v>211.0033213661671</v>
       </c>
       <c r="D48">
-        <v>31.97195625305176</v>
+        <v>34.36090850830078</v>
       </c>
       <c r="E48">
         <v>25.27869677441049</v>
       </c>
       <c r="F48">
-        <v>2.846347808837891</v>
+        <v>2.648454666137695</v>
       </c>
       <c r="G48">
         <v>0.2381323032010778</v>
@@ -1787,7 +1787,7 @@
         <v>9.671196658366</v>
       </c>
       <c r="I48">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1798,16 +1798,16 @@
         <v>47</v>
       </c>
       <c r="C49">
-        <v>160.491964208273</v>
+        <v>158.6195727532088</v>
       </c>
       <c r="D49">
-        <v>42.92282867431641</v>
+        <v>42.83965682983398</v>
       </c>
       <c r="E49">
         <v>710.8830771958565</v>
       </c>
       <c r="F49">
-        <v>59.62279510498047</v>
+        <v>59.73854827880859</v>
       </c>
       <c r="G49">
         <v>-2.316807924352409</v>
@@ -1816,7 +1816,7 @@
         <v>6.329466394030306</v>
       </c>
       <c r="I49">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1845,7 +1845,7 @@
         <v>8.616249065587811</v>
       </c>
       <c r="I50">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1874,7 +1874,7 @@
         <v>9.478193265144439</v>
       </c>
       <c r="I51">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1885,16 +1885,16 @@
         <v>50</v>
       </c>
       <c r="C52">
-        <v>230.7670644194769</v>
+        <v>195.7068689763964</v>
       </c>
       <c r="D52">
-        <v>26.49566078186035</v>
+        <v>24.28691864013672</v>
       </c>
       <c r="E52">
         <v>435.5356769315731</v>
       </c>
       <c r="F52">
-        <v>59.17679595947266</v>
+        <v>64.55855560302734</v>
       </c>
       <c r="G52">
         <v>1.974519515110574</v>
@@ -1903,7 +1903,7 @@
         <v>6.773746381148227</v>
       </c>
       <c r="I52">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1914,16 +1914,16 @@
         <v>51</v>
       </c>
       <c r="C53">
-        <v>113.8851179867005</v>
+        <v>120.9463016958906</v>
       </c>
       <c r="D53">
-        <v>48.54358673095703</v>
+        <v>48.18379592895508</v>
       </c>
       <c r="E53">
         <v>1558.661065889315</v>
       </c>
       <c r="F53">
-        <v>115.5905380249023</v>
+        <v>116.4536666870117</v>
       </c>
       <c r="G53">
         <v>-4.645913252401428</v>
@@ -1932,7 +1932,7 @@
         <v>9.100209265993705</v>
       </c>
       <c r="I53">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -1943,16 +1943,16 @@
         <v>52</v>
       </c>
       <c r="C54">
-        <v>241.7235016684445</v>
+        <v>196.3067975683373</v>
       </c>
       <c r="D54">
-        <v>27.13228797912598</v>
+        <v>24.25494575500488</v>
       </c>
       <c r="E54">
         <v>755.2700581801146</v>
       </c>
       <c r="F54">
-        <v>100.2116775512695</v>
+        <v>112.0997085571289</v>
       </c>
       <c r="G54">
         <v>2.031562830371228</v>
@@ -1961,7 +1961,7 @@
         <v>8.803832620215976</v>
       </c>
       <c r="I54">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -1972,16 +1972,16 @@
         <v>53</v>
       </c>
       <c r="C55">
-        <v>151.3750809182409</v>
+        <v>148.7838284906937</v>
       </c>
       <c r="D55">
-        <v>43.57570266723633</v>
+        <v>43.4605827331543</v>
       </c>
       <c r="E55">
         <v>1264.899823143351</v>
       </c>
       <c r="F55">
-        <v>104.4994964599609</v>
+        <v>104.7762985229492</v>
       </c>
       <c r="G55">
         <v>-2.706180481819132</v>
@@ -1990,7 +1990,7 @@
         <v>2.715786035652243</v>
       </c>
       <c r="I55">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2019,7 +2019,7 @@
         <v>-0.9691183484051571</v>
       </c>
       <c r="I56">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2030,16 +2030,16 @@
         <v>55</v>
       </c>
       <c r="C57">
-        <v>199.4627026402702</v>
+        <v>198.1180756138675</v>
       </c>
       <c r="D57">
-        <v>34.32258605957031</v>
+        <v>34.23759460449219</v>
       </c>
       <c r="E57">
         <v>25.59575949009377</v>
       </c>
       <c r="F57">
-        <v>2.684667587280273</v>
+        <v>2.691332101821899</v>
       </c>
       <c r="G57">
         <v>-0.1671179263512283</v>
@@ -2048,7 +2048,7 @@
         <v>-1.836499198479489</v>
       </c>
       <c r="I57">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2059,16 +2059,16 @@
         <v>56</v>
       </c>
       <c r="C58">
-        <v>205.6830919257723</v>
+        <v>207.0759938260275</v>
       </c>
       <c r="D58">
-        <v>33.40991973876953</v>
+        <v>33.49795532226562</v>
       </c>
       <c r="E58">
         <v>12.64423606528362</v>
       </c>
       <c r="F58">
-        <v>1.362447023391724</v>
+        <v>1.358866453170776</v>
       </c>
       <c r="G58">
         <v>0.0996391493335807</v>
@@ -2077,7 +2077,7 @@
         <v>-1.530310538753543</v>
       </c>
       <c r="I58">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2088,16 +2088,16 @@
         <v>57</v>
       </c>
       <c r="C59">
-        <v>202.2231268443722</v>
+        <v>203.5953581128159</v>
       </c>
       <c r="D59">
-        <v>33.80237197875977</v>
+        <v>33.88910675048828</v>
       </c>
       <c r="E59">
         <v>12.5971306548563</v>
       </c>
       <c r="F59">
-        <v>1.341611981391907</v>
+        <v>1.338178396224976</v>
       </c>
       <c r="G59">
         <v>-0.01533163524593177</v>
@@ -2106,7 +2106,7 @@
         <v>-1.223801256598705</v>
       </c>
       <c r="I59">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2117,16 +2117,16 @@
         <v>58</v>
       </c>
       <c r="C60">
-        <v>201.6663910932875</v>
+        <v>204.4273282870913</v>
       </c>
       <c r="D60">
-        <v>33.52884674072266</v>
+        <v>33.70335388183594</v>
       </c>
       <c r="E60">
         <v>23.20820445037316</v>
       </c>
       <c r="F60">
-        <v>2.491870164871216</v>
+        <v>2.478967905044556</v>
       </c>
       <c r="G60">
         <v>0.03034269269324871</v>
@@ -2135,7 +2135,7 @@
         <v>-1.305201694265891</v>
       </c>
       <c r="I60">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2146,16 +2146,16 @@
         <v>59</v>
       </c>
       <c r="C61">
-        <v>200.858100719646</v>
+        <v>202.2166817268425</v>
       </c>
       <c r="D61">
-        <v>34.04834747314453</v>
+        <v>34.13421630859375</v>
       </c>
       <c r="E61">
         <v>34.456874764448</v>
       </c>
       <c r="F61">
-        <v>3.643194437026978</v>
+        <v>3.634029626846313</v>
       </c>
       <c r="G61">
         <v>-0.09062660158489143</v>
@@ -2164,7 +2164,7 @@
         <v>-1.639802592446514</v>
       </c>
       <c r="I61">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2175,16 +2175,16 @@
         <v>60</v>
       </c>
       <c r="C62">
-        <v>203.6023330876295</v>
+        <v>202.2163097567532</v>
       </c>
       <c r="D62">
-        <v>33.51913452148438</v>
+        <v>33.4315299987793</v>
       </c>
       <c r="E62">
         <v>41.78436304307252</v>
       </c>
       <c r="F62">
-        <v>4.487696170806885</v>
+        <v>4.499456405639648</v>
       </c>
       <c r="G62">
         <v>0.0612476728704989</v>
@@ -2193,7 +2193,7 @@
         <v>-1.095450470097568</v>
       </c>
       <c r="I62">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2222,7 +2222,7 @@
         <v>-1.303367942610337</v>
       </c>
       <c r="I63">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2233,16 +2233,16 @@
         <v>62</v>
       </c>
       <c r="C64">
-        <v>216.1078572446636</v>
+        <v>211.7904898948161</v>
       </c>
       <c r="D64">
-        <v>32.59263229370117</v>
+        <v>32.31975555419922</v>
       </c>
       <c r="E64">
         <v>219.7798828132327</v>
       </c>
       <c r="F64">
-        <v>24.27565765380859</v>
+        <v>24.48061752319336</v>
       </c>
       <c r="G64">
         <v>0.3614021000029659</v>
@@ -2251,7 +2251,7 @@
         <v>-2.996890153055212</v>
       </c>
       <c r="I64">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -2262,16 +2262,16 @@
         <v>63</v>
       </c>
       <c r="C65">
-        <v>158.5796199088042</v>
+        <v>154.364321714714</v>
       </c>
       <c r="D65">
-        <v>43.02151107788086</v>
+        <v>42.83491897583008</v>
       </c>
       <c r="E65">
         <v>570.7407078778269</v>
       </c>
       <c r="F65">
-        <v>47.75904846191406</v>
+        <v>47.96709060668945</v>
       </c>
       <c r="G65">
         <v>-2.819358949109247</v>
@@ -2280,7 +2280,7 @@
         <v>-4.047118092241034</v>
       </c>
       <c r="I65">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2291,16 +2291,16 @@
         <v>64</v>
       </c>
       <c r="C66">
-        <v>221.1021279480878</v>
+        <v>219.525338776895</v>
       </c>
       <c r="D66">
-        <v>29.19924736022949</v>
+        <v>29.0995922088623</v>
       </c>
       <c r="E66">
         <v>1701.564347687097</v>
       </c>
       <c r="F66">
-        <v>209.7873229980469</v>
+        <v>210.5057373046875</v>
       </c>
       <c r="G66">
         <v>1.192672554068895</v>
@@ -2309,7 +2309,7 @@
         <v>1.224496329143648</v>
       </c>
       <c r="I66">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2320,16 +2320,16 @@
         <v>65</v>
       </c>
       <c r="C67">
-        <v>159.2816214104639</v>
+        <v>158.3388051963592</v>
       </c>
       <c r="D67">
-        <v>41.8033561706543</v>
+        <v>41.761474609375</v>
       </c>
       <c r="E67">
         <v>1238.094529523736</v>
       </c>
       <c r="F67">
-        <v>106.6215896606445</v>
+        <v>106.728515625</v>
       </c>
       <c r="G67">
         <v>-2.281667608214841</v>
@@ -2338,7 +2338,7 @@
         <v>0.5497540025124052</v>
       </c>
       <c r="I67">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2349,16 +2349,16 @@
         <v>66</v>
       </c>
       <c r="C68">
-        <v>248.4270775001456</v>
+        <v>250.298782372596</v>
       </c>
       <c r="D68">
-        <v>19.86155891418457</v>
+        <v>19.96328163146973</v>
       </c>
       <c r="E68">
         <v>1478.37646889903</v>
       </c>
       <c r="F68">
-        <v>267.9626159667969</v>
+        <v>266.5971984863281</v>
       </c>
       <c r="G68">
         <v>3.513903955135374</v>
@@ -2367,7 +2367,7 @@
         <v>1.309943888990366</v>
       </c>
       <c r="I68">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2378,16 +2378,16 @@
         <v>67</v>
       </c>
       <c r="C69">
-        <v>197.0723971608055</v>
+        <v>185.0658156007322</v>
       </c>
       <c r="D69">
-        <v>37.35625839233398</v>
+        <v>36.68518447875977</v>
       </c>
       <c r="E69">
         <v>292.6010743627921</v>
       </c>
       <c r="F69">
-        <v>28.19778823852539</v>
+        <v>28.71360206604004</v>
       </c>
       <c r="G69">
         <v>-0.9351353751330883</v>
@@ -2396,7 +2396,7 @@
         <v>-4.295350749098601</v>
       </c>
       <c r="I69">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2407,16 +2407,16 @@
         <v>68</v>
       </c>
       <c r="C70">
-        <v>202.6980191035573</v>
+        <v>204.0889081854114</v>
       </c>
       <c r="D70">
-        <v>33.40224456787109</v>
+        <v>33.49015426635742</v>
       </c>
       <c r="E70">
         <v>20.36903480348701</v>
       </c>
       <c r="F70">
-        <v>2.195317268371582</v>
+        <v>2.189554691314697</v>
       </c>
       <c r="G70">
         <v>0.08839089202534364</v>
@@ -2425,7 +2425,7 @@
         <v>-0.4008727633516296</v>
       </c>
       <c r="I70">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -2436,16 +2436,16 @@
         <v>69</v>
       </c>
       <c r="C71">
-        <v>192.6535283566785</v>
+        <v>197.8638764528695</v>
       </c>
       <c r="D71">
-        <v>35.01353073120117</v>
+        <v>35.34284973144531</v>
       </c>
       <c r="E71">
         <v>18.65366707263456</v>
       </c>
       <c r="F71">
-        <v>1.917921543121338</v>
+        <v>1.900050640106201</v>
       </c>
       <c r="G71">
         <v>-0.3949548349024165</v>
@@ -2454,7 +2454,7 @@
         <v>-2.043470506630904</v>
       </c>
       <c r="I71">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -2483,7 +2483,7 @@
         <v>-1.802040962007777</v>
       </c>
       <c r="I72">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -2494,16 +2494,16 @@
         <v>71</v>
       </c>
       <c r="C73">
-        <v>199.4107901252809</v>
+        <v>202.1261596227613</v>
       </c>
       <c r="D73">
-        <v>33.9703369140625</v>
+        <v>34.14196014404297</v>
       </c>
       <c r="E73">
         <v>39.58186892988306</v>
       </c>
       <c r="F73">
-        <v>4.194680690765381</v>
+        <v>4.173594951629639</v>
       </c>
       <c r="G73">
         <v>-0.09555382349409856</v>
@@ -2512,7 +2512,7 @@
         <v>-1.742113006776057</v>
       </c>
       <c r="I73">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -2523,16 +2523,16 @@
         <v>72</v>
       </c>
       <c r="C74">
-        <v>207.6256135072174</v>
+        <v>210.4781257773617</v>
       </c>
       <c r="D74">
-        <v>32.58411026000977</v>
+        <v>32.76440811157227</v>
       </c>
       <c r="E74">
         <v>89.59064185099123</v>
       </c>
       <c r="F74">
-        <v>9.898269653320312</v>
+        <v>9.84380054473877</v>
       </c>
       <c r="G74">
         <v>0.2878333828145256</v>
@@ -2541,7 +2541,7 @@
         <v>-1.56225071611269</v>
       </c>
       <c r="I74">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -2570,7 +2570,7 @@
         <v>-3.364038488402069</v>
       </c>
       <c r="I75">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -2581,16 +2581,16 @@
         <v>74</v>
       </c>
       <c r="C76">
-        <v>201.5585744194662</v>
+        <v>204.3173334986473</v>
       </c>
       <c r="D76">
-        <v>33.38207244873047</v>
+        <v>33.55643463134766</v>
       </c>
       <c r="E76">
         <v>35.79399999910675</v>
       </c>
       <c r="F76">
-        <v>3.860107421875</v>
+        <v>3.840050220489502</v>
       </c>
       <c r="G76">
         <v>0.02429351747549238</v>
@@ -2599,7 +2599,7 @@
         <v>-2.850329613276325</v>
       </c>
       <c r="I76">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -2610,16 +2610,16 @@
         <v>75</v>
       </c>
       <c r="C77">
-        <v>188.6393680438063</v>
+        <v>211.5045572426403</v>
       </c>
       <c r="D77">
-        <v>35.71997451782227</v>
+        <v>36.98584365844727</v>
       </c>
       <c r="E77">
         <v>122.4589308720097</v>
       </c>
       <c r="F77">
-        <v>12.34189414978027</v>
+        <v>11.91948318481445</v>
       </c>
       <c r="G77">
         <v>-0.6813108349116376</v>
@@ -2628,7 +2628,7 @@
         <v>-4.546921201111702</v>
       </c>
       <c r="I77">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -2657,7 +2657,7 @@
         <v>-0.7150572444261751</v>
       </c>
       <c r="I78">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -2668,16 +2668,16 @@
         <v>77</v>
       </c>
       <c r="C79">
-        <v>199.0121265846156</v>
+        <v>197.6720053187694</v>
       </c>
       <c r="D79">
-        <v>34.68062973022461</v>
+        <v>34.59592819213867</v>
       </c>
       <c r="E79">
         <v>74.4020240477912</v>
       </c>
       <c r="F79">
-        <v>7.723252773284912</v>
+        <v>7.742161750793457</v>
       </c>
       <c r="G79">
         <v>-0.191718887208056</v>
@@ -2686,7 +2686,7 @@
         <v>0.5490306867231698</v>
       </c>
       <c r="I79">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -2715,7 +2715,7 @@
         <v>0.02587660591580461</v>
       </c>
       <c r="I80">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -2726,16 +2726,16 @@
         <v>79</v>
       </c>
       <c r="C81">
-        <v>209.0596094043434</v>
+        <v>196.9424459965014</v>
       </c>
       <c r="D81">
-        <v>34.61347579956055</v>
+        <v>33.84897994995117</v>
       </c>
       <c r="E81">
         <v>75.08637616922351</v>
       </c>
       <c r="F81">
-        <v>7.809412956237793</v>
+        <v>7.985792636871338</v>
       </c>
       <c r="G81">
         <v>-0.1576901133683288</v>
@@ -2744,7 +2744,7 @@
         <v>-4.258154043925821</v>
       </c>
       <c r="I81">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -2755,16 +2755,16 @@
         <v>80</v>
       </c>
       <c r="C82">
-        <v>235.9607523270495</v>
+        <v>234.251144803779</v>
       </c>
       <c r="D82">
-        <v>25.48665428161621</v>
+        <v>25.37860107421875</v>
       </c>
       <c r="E82">
         <v>2427.044252905944</v>
       </c>
       <c r="F82">
-        <v>342.8209228515625</v>
+        <v>344.2805480957031</v>
       </c>
       <c r="G82">
         <v>2.10853553547893</v>
@@ -2773,7 +2773,7 @@
         <v>0.7481270099782461</v>
       </c>
       <c r="I82">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -2784,16 +2784,16 @@
         <v>81</v>
       </c>
       <c r="C83">
-        <v>150.4194953143916</v>
+        <v>154.9152582256754</v>
       </c>
       <c r="D83">
-        <v>42.78627777099609</v>
+        <v>42.98599243164062</v>
       </c>
       <c r="E83">
         <v>3454.663685947395</v>
       </c>
       <c r="F83">
-        <v>290.67236328125</v>
+        <v>289.3218994140625</v>
       </c>
       <c r="G83">
         <v>-2.514697343303455</v>
@@ -2802,7 +2802,7 @@
         <v>3.065985608365474</v>
       </c>
       <c r="I83">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -2813,16 +2813,16 @@
         <v>82</v>
       </c>
       <c r="C84">
-        <v>235.4219415198865</v>
+        <v>233.7345955642441</v>
       </c>
       <c r="D84">
-        <v>25.98773765563965</v>
+        <v>25.88144683837891</v>
       </c>
       <c r="E84">
         <v>490.2055269807897</v>
       </c>
       <c r="F84">
-        <v>67.90663909912109</v>
+        <v>68.18551635742188</v>
       </c>
       <c r="G84">
         <v>1.944243625895261</v>
@@ -2831,7 +2831,7 @@
         <v>-2.419328873481414</v>
       </c>
       <c r="I84">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -2842,16 +2842,16 @@
         <v>83</v>
       </c>
       <c r="C85">
-        <v>186.2819871107802</v>
+        <v>201.7758325287569</v>
       </c>
       <c r="D85">
-        <v>38.12351226806641</v>
+        <v>38.97448348999023</v>
       </c>
       <c r="E85">
         <v>527.239657418635</v>
       </c>
       <c r="F85">
-        <v>49.78719711303711</v>
+        <v>48.70014190673828</v>
       </c>
       <c r="G85">
         <v>-1.340100708621075</v>
@@ -2860,7 +2860,7 @@
         <v>-5.772312393461049</v>
       </c>
       <c r="I85">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>